<commit_message>
Some fix for defect list and commands.js
Some fix for defect list and commands.js
</commit_message>
<xml_diff>
--- a/Defect list.xlsx
+++ b/Defect list.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macintosh/Desktop/weavesock/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macintosh/Desktop/microservicesweave/microservices-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A972F0-8E31-434D-A63F-32F14A2C8B03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC356E8-D960-3742-A6BA-18A6A09D11D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="500" windowWidth="25000" windowHeight="14540" xr2:uid="{D9070192-3944-AE46-8453-8BF5E843F42C}"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="25000" windowHeight="14540" xr2:uid="{D9070192-3944-AE46-8453-8BF5E843F42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sayfa4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sayfa2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sayfa6" sheetId="6" r:id="rId2"/>
+    <sheet name="Sayfa5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sayfa4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sayfa3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sayfa2" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>Defect</t>
   </si>
@@ -187,6 +189,48 @@
   </si>
   <si>
     <t>Go to the login page and create user with a non-alphabetic character name and lastname</t>
+  </si>
+  <si>
+    <t>Creating address with wrong city,postcode and country</t>
+  </si>
+  <si>
+    <t>Using wrong details on address section</t>
+  </si>
+  <si>
+    <t>click address change link and enter non-valid informations</t>
+  </si>
+  <si>
+    <t>Please enter a valid city , postcode etc.</t>
+  </si>
+  <si>
+    <t>Wrong credit card information</t>
+  </si>
+  <si>
+    <t>Using wrong card details on payment section</t>
+  </si>
+  <si>
+    <t>click payment change link and enter non-valid informations</t>
+  </si>
+  <si>
+    <t>Please enter a valid card informations</t>
+  </si>
+  <si>
+    <t>lastname: 7676yyt</t>
+  </si>
+  <si>
+    <t>empty name</t>
+  </si>
+  <si>
+    <t>empty email</t>
+  </si>
+  <si>
+    <t>empty password</t>
+  </si>
+  <si>
+    <t>city : 4545 , etc</t>
+  </si>
+  <si>
+    <t>card number : gkfjgkf</t>
   </si>
 </sst>
 </file>
@@ -487,6 +531,116 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Resim 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A299F2C-9EF1-F04A-8AA5-B0BF59A1F8E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3556000" cy="4597400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Resim 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6044C202-EE6E-ED45-8699-B91441FCEFCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3721100" cy="6654800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>23</xdr:row>
@@ -532,7 +686,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -587,7 +741,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -942,7 +1096,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1205,9 @@
       <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
@@ -1097,7 +1253,9 @@
       <c r="C4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1143,7 +1301,9 @@
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
@@ -1189,7 +1349,9 @@
       <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1325,40 +1487,96 @@
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1636,12 +1854,40 @@
     <hyperlink ref="F6" location="Sayfa3!A1" display="bugss" xr:uid="{B4F57597-0193-1041-97E6-3B91278D6EAF}"/>
     <hyperlink ref="F7" location="Sayfa3!A1" display="bugss" xr:uid="{842FA4F5-D484-8E4D-AE9C-2A696DED9BAA}"/>
     <hyperlink ref="F8" location="Sayfa4!A1" display="bugss" xr:uid="{57D8063D-A3C0-6F4C-B192-0E320D82E559}"/>
+    <hyperlink ref="F9" location="Sayfa5!A1" display="bugss" xr:uid="{A4330D6D-7AD6-D24B-8D83-DE38E3987F00}"/>
+    <hyperlink ref="F10" location="Sayfa6!A1" display="bugss" xr:uid="{21B53A4D-639C-3147-82DB-664B1E4A959F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD8749E-CD56-2343-8AC5-687221DB20D7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF182DED-6C6F-5A4D-8913-141FBA097A6B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7349CE-4AE9-554F-8FF8-AB104C1DF3C9}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1654,7 +1900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD5E29B-8A8F-BE4D-BF79-36B3D125CE84}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1667,7 +1913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1F1895-4A8A-A849-A745-76E27D196A26}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>